<commit_message>
compile daily bond yield data
</commit_message>
<xml_diff>
--- a/paper/revision-tasks.xlsx
+++ b/paper/revision-tasks.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Reviewer</t>
   </si>
@@ -158,9 +157,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Doneish</t>
   </si>
   <si>
     <t>Not Done</t>
@@ -510,7 +506,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,7 +805,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>